<commit_message>
Story node Start dialog v2.00
</commit_message>
<xml_diff>
--- a/_Story/Story.xlsx
+++ b/_Story/Story.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="282">
   <si>
     <t>Center</t>
   </si>
@@ -865,6 +865,9 @@
   </si>
   <si>
     <t>Function</t>
+  </si>
+  <si>
+    <t>https://disk.yandex.ru/d/QfKcuJ_-vLaBZQ</t>
   </si>
 </sst>
 </file>
@@ -1866,10 +1869,10 @@
   <dimension ref="A1:J175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1917,7 +1920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="246" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="315" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -2331,6 +2334,9 @@
       </c>
       <c r="G29" s="18" t="s">
         <v>17</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Smooth loading of scenes start
</commit_message>
<xml_diff>
--- a/_Story/Story.xlsx
+++ b/_Story/Story.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Act1" sheetId="1" r:id="rId1"/>
@@ -1832,7 +1832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -4515,12 +4515,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
New canvas layer system
</commit_message>
<xml_diff>
--- a/_Story/Story.xlsx
+++ b/_Story/Story.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="270">
   <si>
     <t>Center</t>
   </si>
@@ -460,9 +460,6 @@
   </si>
   <si>
     <t>А он точно сможет принять у меня экзамен? У него всё в порядке с...? Ну, то есть, он в своем уме?</t>
-  </si>
-  <si>
-    <t>А сэр Гра… Гру… Слушай, а тебе не кажется, что признести егог имя - уже целое испытание?</t>
   </si>
   <si>
     <t>Позвольте… Так Вы - наш основатель? В наших старинных свёртках ваше имя записано по-другому. Вас все знают под именем Рофар.</t>
@@ -832,6 +829,9 @@
   </si>
   <si>
     <t>Choice</t>
+  </si>
+  <si>
+    <t>А сэр Гра… Гру… Слушай, а тебе не кажется, что признести его имя - уже целое испытание?</t>
   </si>
 </sst>
 </file>
@@ -1836,7 +1836,7 @@
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="H147" sqref="H147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,13 +1854,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>248</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>249</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>4</v>
@@ -1889,19 +1889,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H2" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="I2" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>246</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1909,7 +1909,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>2</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>2</v>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C21" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>2</v>
@@ -2196,7 +2196,7 @@
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>1</v>
@@ -2208,7 +2208,7 @@
         <v>17</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2247,7 +2247,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>0</v>
@@ -2256,12 +2256,12 @@
         <v>14</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C26" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>0</v>
@@ -2303,7 +2303,7 @@
         <v>17</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2600,7 +2600,7 @@
         <v>14</v>
       </c>
       <c r="H50" s="18" t="s">
-        <v>148</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -2613,7 +2613,7 @@
         <v>14</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="26" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2633,7 +2633,7 @@
         <v>18</v>
       </c>
       <c r="H52" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2653,7 +2653,7 @@
         <v>18</v>
       </c>
       <c r="H53" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J53" s="26" t="s">
         <v>47</v>
@@ -2676,7 +2676,7 @@
         <v>18</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2693,7 +2693,7 @@
         <v>14</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -2768,7 +2768,7 @@
         <v>18</v>
       </c>
       <c r="H61" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -2779,7 +2779,7 @@
         <v>18</v>
       </c>
       <c r="H62" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -2789,9 +2789,6 @@
       <c r="D63" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G63" s="18" t="s">
-        <v>14</v>
-      </c>
       <c r="H63" s="18" t="s">
         <v>52</v>
       </c>
@@ -2807,7 +2804,7 @@
         <v>18</v>
       </c>
       <c r="H64" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2816,9 +2813,6 @@
       <c r="D65" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G65" s="18" t="s">
-        <v>14</v>
-      </c>
       <c r="H65" s="18" t="s">
         <v>53</v>
       </c>
@@ -2837,7 +2831,7 @@
         <v>18</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -2900,7 +2894,7 @@
         <v>18</v>
       </c>
       <c r="H71" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="28" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2917,7 +2911,7 @@
         <v>18</v>
       </c>
       <c r="H72" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2928,7 +2922,7 @@
         <v>18</v>
       </c>
       <c r="H73" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2939,7 +2933,7 @@
         <v>18</v>
       </c>
       <c r="H74" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2953,7 +2947,7 @@
         <v>14</v>
       </c>
       <c r="H75" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -2967,7 +2961,7 @@
         <v>18</v>
       </c>
       <c r="H76" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -2981,7 +2975,7 @@
         <v>14</v>
       </c>
       <c r="H77" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2995,7 +2989,7 @@
         <v>18</v>
       </c>
       <c r="H78" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3012,7 +3006,7 @@
         <v>18</v>
       </c>
       <c r="H79" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3076,7 +3070,7 @@
         <v>18</v>
       </c>
       <c r="H84" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3109,7 +3103,7 @@
         <v>18</v>
       </c>
       <c r="H87" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -3125,7 +3119,7 @@
     </row>
     <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="G89" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H89" s="18" t="s">
         <v>64</v>
@@ -3142,15 +3136,15 @@
         <v>14</v>
       </c>
       <c r="H90" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="G91" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H91" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -3164,12 +3158,12 @@
         <v>18</v>
       </c>
       <c r="H92" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="G93" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H93" s="18" t="s">
         <v>79</v>
@@ -3200,7 +3194,7 @@
         <v>14</v>
       </c>
       <c r="H95" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3244,10 +3238,10 @@
     </row>
     <row r="99" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="G99" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H99" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -3266,7 +3260,7 @@
         <v>17</v>
       </c>
       <c r="C101" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D101" s="18" t="s">
         <v>2</v>
@@ -3283,7 +3277,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C102" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D102" s="18" t="s">
         <v>1</v>
@@ -3309,7 +3303,7 @@
         <v>14</v>
       </c>
       <c r="H103" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3323,7 +3317,7 @@
         <v>14</v>
       </c>
       <c r="H104" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3336,10 +3330,10 @@
         <v>35</v>
       </c>
       <c r="G105" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H105" s="30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3347,16 +3341,16 @@
         <v>20</v>
       </c>
       <c r="C106" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D106" s="29"/>
       <c r="E106" s="29"/>
       <c r="F106" s="29"/>
       <c r="G106" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H106" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -3364,16 +3358,16 @@
         <v>21</v>
       </c>
       <c r="C107" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D107" s="29"/>
       <c r="E107" s="29"/>
       <c r="F107" s="29"/>
       <c r="G107" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H107" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -3381,7 +3375,7 @@
       <c r="E108" s="29"/>
       <c r="F108" s="29"/>
       <c r="G108" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H108" s="30" t="s">
         <v>88</v>
@@ -3389,48 +3383,48 @@
     </row>
     <row r="109" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B109" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G109" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H109" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B110" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G110" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H110" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G111" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H111" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="G112" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H112" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="G113" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H113" s="30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -3458,7 +3452,7 @@
         <v>26</v>
       </c>
       <c r="H115" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -3472,7 +3466,7 @@
         <v>26</v>
       </c>
       <c r="H116" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -3491,10 +3485,10 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G118" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H118" s="30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -3508,7 +3502,7 @@
         <v>26</v>
       </c>
       <c r="H119" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3516,13 +3510,13 @@
         <v>22</v>
       </c>
       <c r="C120" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G120" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H120" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3533,15 +3527,15 @@
         <v>14</v>
       </c>
       <c r="H121" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="G122" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H122" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3555,26 +3549,26 @@
         <v>26</v>
       </c>
       <c r="H123" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C124" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G124" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H124" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="G125" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H125" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -3608,7 +3602,7 @@
         <v>14</v>
       </c>
       <c r="H127" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -3616,18 +3610,18 @@
         <v>14</v>
       </c>
       <c r="H128" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C129" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G129" s="18" t="s">
         <v>14</v>
       </c>
       <c r="H129" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -3675,7 +3669,7 @@
         <v>14</v>
       </c>
       <c r="H132" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -3689,7 +3683,7 @@
         <v>18</v>
       </c>
       <c r="H133" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3703,7 +3697,7 @@
         <v>18</v>
       </c>
       <c r="H134" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3720,7 +3714,7 @@
         <v>14</v>
       </c>
       <c r="H135" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -3739,35 +3733,35 @@
     </row>
     <row r="137" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B137" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G137" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H137" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B138" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G138" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H138" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B139" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G139" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H139" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -3775,13 +3769,13 @@
         <v>1</v>
       </c>
       <c r="F140" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G140" s="18" t="s">
         <v>14</v>
       </c>
       <c r="H140" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -3792,7 +3786,7 @@
         <v>14</v>
       </c>
       <c r="H141" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -3806,7 +3800,7 @@
         <v>18</v>
       </c>
       <c r="H142" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -3814,13 +3808,13 @@
         <v>1</v>
       </c>
       <c r="F143" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G143" s="18" t="s">
         <v>14</v>
       </c>
       <c r="H143" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="144" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3834,7 +3828,7 @@
         <v>18</v>
       </c>
       <c r="H144" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="145" spans="4:8" ht="60" x14ac:dyDescent="0.25">
@@ -3842,21 +3836,21 @@
         <v>1</v>
       </c>
       <c r="F145" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G145" s="18" t="s">
         <v>14</v>
       </c>
       <c r="H145" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="146" spans="4:8" ht="75" x14ac:dyDescent="0.25">
       <c r="G146" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H146" s="28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="147" spans="4:8" x14ac:dyDescent="0.25">
@@ -3870,7 +3864,7 @@
         <v>14</v>
       </c>
       <c r="H147" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="148" spans="4:8" ht="30" x14ac:dyDescent="0.25">
@@ -3884,7 +3878,7 @@
         <v>14</v>
       </c>
       <c r="H148" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="149" spans="4:8" ht="45" x14ac:dyDescent="0.25">
@@ -3898,7 +3892,7 @@
         <v>18</v>
       </c>
       <c r="H149" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="150" spans="4:8" x14ac:dyDescent="0.25">
@@ -3906,7 +3900,7 @@
         <v>18</v>
       </c>
       <c r="H150" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="151" spans="4:8" ht="45" x14ac:dyDescent="0.25">
@@ -3920,7 +3914,7 @@
         <v>14</v>
       </c>
       <c r="H151" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="152" spans="4:8" ht="30" x14ac:dyDescent="0.25">
@@ -3934,7 +3928,7 @@
         <v>18</v>
       </c>
       <c r="H152" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="153" spans="4:8" x14ac:dyDescent="0.25">
@@ -3948,7 +3942,7 @@
         <v>14</v>
       </c>
       <c r="H153" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="154" spans="4:8" ht="60" x14ac:dyDescent="0.25">
@@ -3962,7 +3956,7 @@
         <v>18</v>
       </c>
       <c r="H154" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="155" spans="4:8" x14ac:dyDescent="0.25">
@@ -3976,7 +3970,7 @@
         <v>14</v>
       </c>
       <c r="H155" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="156" spans="4:8" x14ac:dyDescent="0.25">
@@ -3984,7 +3978,7 @@
         <v>14</v>
       </c>
       <c r="H156" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="157" spans="4:8" ht="30" x14ac:dyDescent="0.25">
@@ -3998,7 +3992,7 @@
         <v>18</v>
       </c>
       <c r="H157" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="158" spans="4:8" x14ac:dyDescent="0.25">
@@ -4006,7 +4000,7 @@
         <v>18</v>
       </c>
       <c r="H158" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="159" spans="4:8" ht="30" x14ac:dyDescent="0.25">
@@ -4020,7 +4014,7 @@
         <v>18</v>
       </c>
       <c r="H159" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="160" spans="4:8" x14ac:dyDescent="0.25">
@@ -4028,13 +4022,13 @@
         <v>1</v>
       </c>
       <c r="F160" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G160" s="18" t="s">
         <v>14</v>
       </c>
       <c r="H160" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="161" spans="2:8" x14ac:dyDescent="0.25">
@@ -4042,7 +4036,7 @@
         <v>14</v>
       </c>
       <c r="H161" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="162" spans="2:8" x14ac:dyDescent="0.25">
@@ -4056,7 +4050,7 @@
         <v>14</v>
       </c>
       <c r="H162" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="163" spans="2:8" x14ac:dyDescent="0.25">
@@ -4064,13 +4058,13 @@
         <v>2</v>
       </c>
       <c r="F163" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G163" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H163" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="164" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -4078,7 +4072,7 @@
         <v>18</v>
       </c>
       <c r="H164" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="165" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -4092,7 +4086,7 @@
         <v>14</v>
       </c>
       <c r="H165" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="166" spans="2:8" x14ac:dyDescent="0.25">
@@ -4100,13 +4094,13 @@
         <v>2</v>
       </c>
       <c r="F166" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G166" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H166" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="167" spans="2:8" x14ac:dyDescent="0.25">
@@ -4114,7 +4108,7 @@
         <v>18</v>
       </c>
       <c r="H167" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="168" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -4122,29 +4116,29 @@
         <v>14</v>
       </c>
       <c r="H168" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="169" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B169" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G169" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H169" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="170" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B170" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G170" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H170" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="171" spans="2:8" ht="75" x14ac:dyDescent="0.25">
@@ -4158,7 +4152,7 @@
         <v>18</v>
       </c>
       <c r="H171" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="172" spans="2:8" x14ac:dyDescent="0.25">
@@ -4172,7 +4166,7 @@
         <v>14</v>
       </c>
       <c r="H172" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="173" spans="2:8" x14ac:dyDescent="0.25">
@@ -4183,7 +4177,7 @@
         <v>14</v>
       </c>
       <c r="H173" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="174" spans="2:8" ht="75" x14ac:dyDescent="0.25">
@@ -4197,7 +4191,7 @@
         <v>18</v>
       </c>
       <c r="H174" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="175" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -4205,7 +4199,7 @@
         <v>18</v>
       </c>
       <c r="H175" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -4540,13 +4534,13 @@
         <v>16</v>
       </c>
       <c r="F1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H1" t="s">
         <v>258</v>
       </c>
-      <c r="H1" t="s">
-        <v>259</v>
-      </c>
       <c r="I1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4560,16 +4554,16 @@
         <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4583,16 +4577,16 @@
         <v>66</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -4609,13 +4603,13 @@
         <v>14</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4629,7 +4623,7 @@
         <v>17</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4643,7 +4637,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4802,18 +4796,18 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" t="s">
         <v>201</v>
-      </c>
-      <c r="C23" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>228</v>
+      </c>
+      <c r="C24" t="s">
         <v>229</v>
-      </c>
-      <c r="C24" t="s">
-        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Help Book in Story inplement
</commit_message>
<xml_diff>
--- a/_Story/Story.xlsx
+++ b/_Story/Story.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="272">
   <si>
     <t>Center</t>
   </si>
@@ -832,6 +832,12 @@
   </si>
   <si>
     <t>А сэр Гра… Гру… Слушай, а тебе не кажется, что признести его имя - уже целое испытание?</t>
+  </si>
+  <si>
+    <t>HelpBook</t>
+  </si>
+  <si>
+    <t>Даёт доступ к книге подсказке</t>
   </si>
 </sst>
 </file>
@@ -1421,7 +1427,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1484,6 +1490,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1830,13 +1842,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J175"/>
+  <dimension ref="A1:J177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H147" sqref="H147"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1966,108 +1978,86 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="D7" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="18" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="H7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="D8" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="22" t="s">
+      <c r="G8" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="22" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="D8" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="D9" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="D10" s="18" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="D11" s="18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D12" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" s="18" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
       <c r="G13" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>12</v>
+      <c r="H13" s="22" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2075,13 +2065,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>114</v>
+        <v>35</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="18" t="s">
-        <v>126</v>
+      <c r="H14" s="22" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2089,33 +2079,36 @@
         <v>2</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>20</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>127</v>
+        <v>113</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="J15" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="D17" s="18" t="s">
         <v>2</v>
       </c>
@@ -2126,63 +2119,63 @@
         <v>20</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="J17" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="s">
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="D18" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D19" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="18" t="s">
+      <c r="D20" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H20" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="J18" s="18" t="s">
+      <c r="J20" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="D19" s="18" t="s">
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="D21" s="18" t="s">
         <v>0</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="D20" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>2</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>46</v>
@@ -2191,92 +2184,95 @@
         <v>14</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="21" t="s">
-        <v>268</v>
-      </c>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="D22" s="18" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>17</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
-        <v>3</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C23" s="18" t="s">
+        <v>251</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>2</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>14</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="21" t="s">
+        <v>268</v>
+      </c>
       <c r="D24" s="18" t="s">
         <v>1</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>33</v>
+        <v>118</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>17</v>
       </c>
       <c r="H24" s="18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
+        <v>3</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="D26" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="18" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="23">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="23">
         <v>4</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C27" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="18" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C26" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D27" s="18" t="s">
         <v>0</v>
       </c>
@@ -2284,379 +2280,364 @@
         <v>14</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C28" s="18" t="s">
+        <v>250</v>
+      </c>
       <c r="D28" s="18" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>40</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>14</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D29" s="18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D30" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="18" t="s">
-        <v>33</v>
-      </c>
       <c r="G30" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H30" s="18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D31" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="G31" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="18" t="s">
-        <v>135</v>
+      <c r="I31" s="18" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="D32" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D33" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="G32" s="18" t="s">
+      <c r="F33" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="H33" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D34" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="18" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D33" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G33" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" s="18" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D35" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="18" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D34" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F34" s="18" t="s">
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D36" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G34" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" s="18" t="s">
+      <c r="G36" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="18" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="D35" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F35" s="18" t="s">
+    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="D37" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" s="18" t="s">
         <v>34</v>
-      </c>
-      <c r="G35" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D36" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G36" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D37" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>33</v>
       </c>
       <c r="G37" s="18" t="s">
         <v>17</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>39</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D38" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E38" s="18" t="s">
         <v>2</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D39" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" s="18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>141</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D40" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>2</v>
       </c>
       <c r="F40" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D41" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G40" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H40" s="18" t="s">
+      <c r="G41" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D42" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42" s="18" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="G41" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H41" s="18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F42" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G42" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="25"/>
       <c r="C43" s="25"/>
-      <c r="D43" s="18" t="s">
-        <v>1</v>
-      </c>
       <c r="G43" s="18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="25"/>
       <c r="C44" s="25"/>
       <c r="D44" s="18" t="s">
         <v>1</v>
       </c>
+      <c r="F44" s="18" t="s">
+        <v>33</v>
+      </c>
       <c r="G44" s="18" t="s">
         <v>17</v>
       </c>
       <c r="H44" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="26" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F45" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G45" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H45" s="26" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F46" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="G46" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" s="26" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="20"/>
       <c r="B47" s="21"/>
       <c r="C47" s="20"/>
       <c r="D47" s="26" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>2</v>
       </c>
       <c r="F47" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47" s="26" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="20"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="G47" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H47" s="26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F48" s="26" t="s">
-        <v>40</v>
-      </c>
       <c r="G48" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H48" s="26" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="18" t="s">
-        <v>1</v>
+    </row>
+    <row r="49" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F49" s="26" t="s">
+        <v>41</v>
       </c>
       <c r="G49" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H49" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="H49" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="25"/>
+      <c r="B50" s="21"/>
       <c r="C50" s="25"/>
-      <c r="D50" s="18" t="s">
-        <v>2</v>
+      <c r="D50" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="26" t="s">
+        <v>40</v>
       </c>
       <c r="G50" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H50" s="18" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H50" s="26" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="25"/>
       <c r="C51" s="25"/>
       <c r="D51" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H51" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" s="18" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H53" s="18" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" s="26" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F52" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="G52" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H52" s="26" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="27"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F53" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G53" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H53" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="J53" s="26" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="26" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2670,55 +2651,76 @@
         <v>2</v>
       </c>
       <c r="F54" s="26" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G54" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H54" s="26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="27"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G55" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="J55" s="26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="26" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="20"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H56" s="26" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
-      <c r="B55" s="21"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F55" s="26" t="s">
+    <row r="57" spans="1:10" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="20"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="G55" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H55" s="26" t="s">
+      <c r="G57" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" s="26" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D56" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G56" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H56" s="18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D57" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G57" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D58" s="18" t="s">
         <v>1</v>
       </c>
@@ -2726,153 +2728,153 @@
         <v>17</v>
       </c>
       <c r="H58" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="20">
-        <v>5</v>
-      </c>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D59" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F59" s="18" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>1</v>
       </c>
       <c r="G59" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H59" s="18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="D60" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="G60" s="18" t="s">
         <v>17</v>
       </c>
+      <c r="H60" s="18" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="20">
+        <v>5</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G61" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G62" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="20">
         <v>6</v>
       </c>
-      <c r="D61" s="18" t="s">
+      <c r="D63" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E61" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F61" s="18" t="s">
+      <c r="E63" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F63" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="G61" s="18" t="s">
+      <c r="G63" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H61" s="18" t="s">
+      <c r="H63" s="18" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D62" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G62" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H62" s="18" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="20">
-        <v>7</v>
-      </c>
-      <c r="D63" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H63" s="18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D64" s="18" t="s">
         <v>1</v>
-      </c>
-      <c r="F64" s="18" t="s">
-        <v>35</v>
       </c>
       <c r="G64" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H64" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
-      <c r="C65" s="23"/>
+      <c r="A65" s="20">
+        <v>7</v>
+      </c>
       <c r="D65" s="18" t="s">
         <v>2</v>
       </c>
       <c r="H65" s="18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A66" s="20">
-        <v>8</v>
-      </c>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D66" s="18" t="s">
         <v>1</v>
       </c>
       <c r="F66" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G66" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
-      <c r="C67" s="18"/>
+      <c r="A67" s="23"/>
+      <c r="C67" s="23"/>
       <c r="D67" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G67" s="18" t="s">
-        <v>14</v>
-      </c>
       <c r="H67" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A68" s="20">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>1</v>
+      </c>
+      <c r="F68" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="G68" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H68" s="18" t="s">
-        <v>55</v>
+        <v>156</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="20">
-        <v>10</v>
-      </c>
+      <c r="A69" s="18"/>
+      <c r="C69" s="18"/>
       <c r="D69" s="18" t="s">
         <v>2</v>
       </c>
       <c r="G69" s="18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H69" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="20">
+        <v>9</v>
+      </c>
       <c r="D70" s="18" t="s">
         <v>1</v>
       </c>
@@ -2880,80 +2882,74 @@
         <v>18</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="20">
+        <v>10</v>
+      </c>
       <c r="D71" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F71" s="18" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="G71" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H71" s="18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" s="28" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="20"/>
-      <c r="D72" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="F72" s="28" t="s">
-        <v>56</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D72" s="18" t="s">
+        <v>1</v>
       </c>
       <c r="G72" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H72" s="28" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H72" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D73" s="18" t="s">
         <v>1</v>
+      </c>
+      <c r="F73" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="G73" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H73" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="D74" s="18" t="s">
-        <v>1</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="28" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A74" s="20"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="F74" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="G74" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H74" s="18" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="H74" s="28" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D75" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F75" s="18" t="s">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="G75" s="18" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H75" s="18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A76" s="20">
-        <v>11</v>
-      </c>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="D76" s="18" t="s">
         <v>1</v>
       </c>
@@ -2961,26 +2957,26 @@
         <v>18</v>
       </c>
       <c r="H76" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="D77" s="18" t="s">
         <v>2</v>
       </c>
       <c r="F77" s="18" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="G77" s="18" t="s">
         <v>14</v>
       </c>
       <c r="H77" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" s="20">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D78" s="18" t="s">
         <v>1</v>
@@ -2989,296 +2985,290 @@
         <v>18</v>
       </c>
       <c r="H78" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="D79" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F79" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G79" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H79" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>12</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G80" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H80" s="18" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="20">
+    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
         <v>13</v>
       </c>
-      <c r="D79" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F79" s="18" t="s">
+      <c r="D81" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F81" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G79" s="18" t="s">
+      <c r="G81" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H79" s="18" t="s">
+      <c r="H81" s="18" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="20">
-        <v>14</v>
-      </c>
-      <c r="D80" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F80" s="18" t="s">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>14</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F82" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="G80" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A81" s="20">
+      <c r="G82" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
         <v>15</v>
       </c>
-      <c r="H81" s="18" t="s">
+      <c r="H83" s="18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D82" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G82" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H82" s="18" t="s">
+    <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D84" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G84" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H84" s="18" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D83" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F83" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G83" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H83" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="20">
-        <v>16</v>
-      </c>
-      <c r="D84" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F84" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="G84" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H84" s="18" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D85" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F85" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="G85" s="18" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H85" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="20">
+        <v>16</v>
+      </c>
+      <c r="D86" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F86" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G86" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H86" s="18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D87" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G87" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H87" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="G86" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H86" s="18" t="s">
+    <row r="88" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="G88" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H88" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="D87" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F87" s="18" t="s">
+    <row r="89" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D89" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F89" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G87" s="18" t="s">
+      <c r="G89" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H87" s="18" t="s">
+      <c r="H89" s="18" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D88" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G88" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H88" s="18" t="s">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D90" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G90" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H90" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="G89" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="H89" s="18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D90" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F90" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="G90" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H90" s="18" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="G91" s="18" t="s">
         <v>255</v>
       </c>
       <c r="H91" s="18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D92" s="18" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F92" s="18" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="G92" s="18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H92" s="18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="G93" s="18" t="s">
         <v>255</v>
       </c>
       <c r="H93" s="18" t="s">
-        <v>79</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D94" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" s="18" t="s">
         <v>35</v>
       </c>
       <c r="G94" s="18" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H94" s="18" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D95" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F95" s="18" t="s">
-        <v>81</v>
-      </c>
       <c r="G95" s="18" t="s">
-        <v>14</v>
+        <v>255</v>
       </c>
       <c r="H95" s="18" t="s">
-        <v>171</v>
+        <v>79</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D96" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E96" s="18" t="s">
         <v>2</v>
       </c>
       <c r="F96" s="18" t="s">
         <v>35</v>
       </c>
       <c r="G96" s="18" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="H96" s="18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D97" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F97" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G97" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H97" s="18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D98" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E97" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F97" s="18" t="s">
+      <c r="E98" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F98" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G97" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="H97" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G98" s="18" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H98" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D99" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F99" s="18" t="s">
+        <v>35</v>
+      </c>
       <c r="G99" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="H99" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G100" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G101" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="H99" s="18" t="s">
+      <c r="H101" s="18" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D100" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F100" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G100" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="20">
-        <v>17</v>
-      </c>
-      <c r="C101" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="D101" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F101" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G101" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H101" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C102" s="18" t="s">
-        <v>252</v>
-      </c>
       <c r="D102" s="18" t="s">
         <v>1</v>
       </c>
@@ -3288,11 +3278,14 @@
       <c r="G102" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H102" s="18" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="20">
+        <v>17</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>250</v>
+      </c>
       <c r="D103" s="18" t="s">
         <v>2</v>
       </c>
@@ -3303,74 +3296,77 @@
         <v>14</v>
       </c>
       <c r="H103" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C104" s="18" t="s">
+        <v>252</v>
+      </c>
       <c r="D104" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F104" s="18" t="s">
         <v>35</v>
       </c>
       <c r="G104" s="18" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H104" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D105" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F105" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G105" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H105" s="18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D106" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F106" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G106" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H106" s="18" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="20">
+    <row r="107" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A107" s="20">
         <v>18</v>
-      </c>
-      <c r="D105" s="29"/>
-      <c r="E105" s="29"/>
-      <c r="F105" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G105" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="H105" s="30" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="20">
-        <v>20</v>
-      </c>
-      <c r="C106" s="18" t="s">
-        <v>253</v>
-      </c>
-      <c r="D106" s="29"/>
-      <c r="E106" s="29"/>
-      <c r="F106" s="29"/>
-      <c r="G106" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="H106" s="30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="20">
-        <v>21</v>
-      </c>
-      <c r="C107" s="18" t="s">
-        <v>252</v>
       </c>
       <c r="D107" s="29"/>
       <c r="E107" s="29"/>
-      <c r="F107" s="29"/>
+      <c r="F107" s="29" t="s">
+        <v>35</v>
+      </c>
       <c r="G107" s="18" t="s">
         <v>254</v>
       </c>
       <c r="H107" s="30" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A108" s="20">
+        <v>20</v>
+      </c>
+      <c r="C108" s="18" t="s">
+        <v>253</v>
+      </c>
       <c r="D108" s="29"/>
       <c r="E108" s="29"/>
       <c r="F108" s="29"/>
@@ -3378,100 +3374,100 @@
         <v>254</v>
       </c>
       <c r="H108" s="30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="20">
+        <v>21</v>
+      </c>
+      <c r="C109" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="D109" s="29"/>
+      <c r="E109" s="29"/>
+      <c r="F109" s="29"/>
+      <c r="G109" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="H109" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D110" s="29"/>
+      <c r="E110" s="29"/>
+      <c r="F110" s="29"/>
+      <c r="G110" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="H110" s="30" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B109" s="21" t="s">
+    <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B111" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="G109" s="18" t="s">
+      <c r="G111" s="18" t="s">
         <v>256</v>
       </c>
-      <c r="H109" s="18" t="s">
+      <c r="H111" s="18" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B110" s="21" t="s">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B112" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="G110" s="18" t="s">
+      <c r="G112" s="18" t="s">
         <v>256</v>
       </c>
-      <c r="H110" s="18" t="s">
+      <c r="H112" s="18" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G111" s="18" t="s">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G113" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="H111" s="18" t="s">
+      <c r="H113" s="18" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="G112" s="18" t="s">
+    <row r="114" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="G114" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="H112" s="30" t="s">
+      <c r="H114" s="30" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="G113" s="18" t="s">
+    <row r="115" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G115" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="H113" s="30" t="s">
+      <c r="H115" s="30" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D114" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F114" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="G114" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H114" s="18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D115" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F115" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="G115" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="H115" s="18" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D116" s="18" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F116" s="18" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="G116" s="18" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H116" s="18" t="s">
-        <v>184</v>
+        <v>91</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D117" s="18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F117" s="18" t="s">
         <v>56</v>
@@ -3480,15 +3476,21 @@
         <v>26</v>
       </c>
       <c r="H117" s="18" t="s">
-        <v>92</v>
+        <v>183</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D118" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F118" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="G118" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="H118" s="30" t="s">
-        <v>185</v>
+        <v>26</v>
+      </c>
+      <c r="H118" s="18" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -3496,166 +3498,157 @@
         <v>0</v>
       </c>
       <c r="F119" s="18" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="G119" s="18" t="s">
         <v>26</v>
       </c>
       <c r="H119" s="18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="20">
-        <v>22</v>
-      </c>
-      <c r="C120" s="18" t="s">
-        <v>250</v>
-      </c>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G120" s="18" t="s">
         <v>254</v>
       </c>
       <c r="H120" s="30" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D121" s="18" t="s">
+        <v>0</v>
+      </c>
       <c r="F121" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G121" s="18" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H121" s="18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="20">
+        <v>22</v>
+      </c>
+      <c r="C122" s="18" t="s">
+        <v>250</v>
+      </c>
       <c r="G122" s="18" t="s">
         <v>254</v>
       </c>
       <c r="H122" s="30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D123" s="18" t="s">
-        <v>0</v>
-      </c>
       <c r="F123" s="18" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G123" s="18" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H123" s="18" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C124" s="18" t="s">
-        <v>251</v>
-      </c>
       <c r="G124" s="18" t="s">
         <v>254</v>
       </c>
       <c r="H124" s="30" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D125" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F125" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G125" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H125" s="18" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C126" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="G126" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="H126" s="30" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="G125" s="18" t="s">
+    <row r="127" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="G127" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="H125" s="30" t="s">
+      <c r="H127" s="30" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D126" s="18" t="s">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D128" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E126" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F126" s="18" t="s">
+      <c r="E128" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F128" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G126" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H126" s="18" t="s">
+      <c r="G128" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H128" s="18" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D127" s="18" t="s">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D129" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E127" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F127" s="18" t="s">
+      <c r="E129" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F129" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G127" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H127" s="18" t="s">
+      <c r="G129" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H129" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G128" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H128" s="18" t="s">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G130" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H130" s="18" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C129" s="20" t="s">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C131" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="G129" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H129" s="18" t="s">
+      <c r="G131" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H131" s="18" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D130" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E130" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F130" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G130" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="20">
-        <v>23</v>
-      </c>
-      <c r="D131" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F131" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G131" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="20">
-        <v>24</v>
-      </c>
       <c r="D132" s="18" t="s">
         <v>1</v>
       </c>
@@ -3668,11 +3661,11 @@
       <c r="G132" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H132" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="20">
+        <v>23</v>
+      </c>
       <c r="D133" s="18" t="s">
         <v>2</v>
       </c>
@@ -3682,78 +3675,87 @@
       <c r="G133" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H133" s="18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="20">
+        <v>24</v>
+      </c>
       <c r="D134" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E134" s="18" t="s">
         <v>2</v>
       </c>
       <c r="F134" s="18" t="s">
         <v>101</v>
       </c>
       <c r="G134" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H134" s="18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="D135" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F135" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G135" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H134" s="18" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="D135" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E135" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F135" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="G135" s="18" t="s">
-        <v>14</v>
-      </c>
       <c r="H135" s="18" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D136" s="18" t="s">
         <v>2</v>
       </c>
       <c r="F136" s="18" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="G136" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H136" s="18" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D137" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E137" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F137" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G137" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H137" s="18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D138" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F138" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G138" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H138" s="18" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B137" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="G137" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="H137" s="18" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B138" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="G138" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="H138" s="18" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B139" s="21" t="s">
         <v>268</v>
       </c>
@@ -3761,77 +3763,71 @@
         <v>256</v>
       </c>
       <c r="H139" s="18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B140" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="G140" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="H140" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B141" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="G141" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="H141" s="18" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D140" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F140" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="G140" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H140" s="18" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D141" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G141" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H141" s="18" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D142" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F142" s="18" t="s">
-        <v>41</v>
+        <v>200</v>
       </c>
       <c r="G142" s="18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H142" s="18" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D143" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F143" s="18" t="s">
-        <v>200</v>
-      </c>
       <c r="G143" s="18" t="s">
         <v>14</v>
       </c>
       <c r="H143" s="18" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D144" s="18" t="s">
         <v>2</v>
       </c>
       <c r="F144" s="18" t="s">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="G144" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H144" s="18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="145" spans="4:8" ht="60" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="145" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D145" s="18" t="s">
         <v>1</v>
       </c>
@@ -3842,121 +3838,121 @@
         <v>14</v>
       </c>
       <c r="H145" s="18" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="146" spans="4:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="D146" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F146" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="G146" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H146" s="18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="147" spans="4:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="D147" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F147" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="G147" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H147" s="18" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="146" spans="4:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="G146" s="18" t="s">
+    <row r="148" spans="4:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="G148" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="H146" s="28" t="s">
+      <c r="H148" s="28" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="147" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D147" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F147" s="18" t="s">
+    <row r="149" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D149" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F149" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="G147" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H147" s="18" t="s">
+      <c r="G149" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H149" s="18" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="148" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D148" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F148" s="18" t="s">
+    <row r="150" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D150" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F150" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="G148" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H148" s="18" t="s">
+      <c r="G150" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H150" s="18" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="149" spans="4:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="D149" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F149" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="G149" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H149" s="18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="150" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G150" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H150" s="18" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="151" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D151" s="18" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F151" s="18" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="G151" s="18" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H151" s="18" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="152" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D152" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F152" s="18" t="s">
-        <v>114</v>
-      </c>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="152" spans="4:8" x14ac:dyDescent="0.25">
       <c r="G152" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H152" s="18" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="153" spans="4:8" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="153" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D153" s="18" t="s">
         <v>1</v>
       </c>
       <c r="F153" s="18" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="G153" s="18" t="s">
         <v>14</v>
       </c>
       <c r="H153" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="154" spans="4:8" ht="60" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="154" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D154" s="18" t="s">
         <v>2</v>
       </c>
       <c r="F154" s="18" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G154" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H154" s="18" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="155" spans="4:8" x14ac:dyDescent="0.25">
@@ -3964,43 +3960,49 @@
         <v>1</v>
       </c>
       <c r="F155" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G155" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H155" s="18" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="156" spans="4:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="D156" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F156" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="G156" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H156" s="18" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="157" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D157" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F157" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G155" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H155" s="18" t="s">
+      <c r="G157" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H157" s="18" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="156" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G156" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H156" s="18" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="157" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D157" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F157" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G157" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H157" s="18" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="158" spans="4:8" x14ac:dyDescent="0.25">
       <c r="G158" s="18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H158" s="18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="159" spans="4:8" ht="30" x14ac:dyDescent="0.25">
@@ -4014,29 +4016,29 @@
         <v>18</v>
       </c>
       <c r="H159" s="18" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="160" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="G160" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H160" s="18" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="161" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D161" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F161" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G161" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H161" s="18" t="s">
         <v>222</v>
-      </c>
-    </row>
-    <row r="160" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D160" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F160" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="G160" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H160" s="18" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="161" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G161" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H161" s="18" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="162" spans="2:8" x14ac:dyDescent="0.25">
@@ -4044,161 +4046,183 @@
         <v>1</v>
       </c>
       <c r="F162" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="G162" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H162" s="18" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="163" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G163" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H163" s="18" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="164" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D164" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F164" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="G162" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H162" s="18" t="s">
+      <c r="G164" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H164" s="18" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="163" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D163" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F163" s="18" t="s">
+    <row r="165" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D165" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F165" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="G163" s="18" t="s">
+      <c r="G165" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H163" s="18" t="s">
+      <c r="H165" s="18" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="164" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="G164" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H164" s="18" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="165" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D165" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F165" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G165" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H165" s="18" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D166" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F166" s="18" t="s">
-        <v>228</v>
-      </c>
+    <row r="166" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="G166" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H166" s="18" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="167" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D167" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F167" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G167" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H167" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="168" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D168" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F168" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="G168" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H168" s="18" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="167" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G167" s="18" t="s">
+    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G169" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H167" s="18" t="s">
+      <c r="H169" s="18" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="168" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="G168" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H168" s="18" t="s">
+    <row r="170" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G170" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H170" s="18" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B169" s="21" t="s">
+    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B171" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="G169" s="18" t="s">
+      <c r="G171" s="18" t="s">
         <v>256</v>
       </c>
-      <c r="H169" s="18" t="s">
+      <c r="H171" s="18" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B170" s="21" t="s">
+    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B172" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="G170" s="18" t="s">
+      <c r="G172" s="18" t="s">
         <v>256</v>
       </c>
-      <c r="H170" s="18" t="s">
+      <c r="H172" s="18" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="171" spans="2:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="D171" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F171" s="18" t="s">
+    <row r="173" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="D173" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F173" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G171" s="18" t="s">
+      <c r="G173" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H171" s="18" t="s">
+      <c r="H173" s="18" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D172" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F172" s="18" t="s">
+    <row r="174" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D174" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F174" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G172" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H172" s="18" t="s">
+      <c r="G174" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H174" s="18" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="173" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F173" s="18" t="s">
+    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F175" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G173" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H173" s="18" t="s">
+      <c r="G175" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H175" s="18" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="174" spans="2:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="D174" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F174" s="18" t="s">
+    <row r="176" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="D176" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F176" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="G174" s="18" t="s">
+      <c r="G176" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H174" s="18" t="s">
+      <c r="H176" s="18" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="175" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="G175" s="18" t="s">
+    <row r="177" spans="7:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G177" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H175" s="18" t="s">
+      <c r="H177" s="18" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4212,25 +4236,31 @@
           <x14:formula1>
             <xm:f>List!$A$3:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D92 D94:D104 D114:D117 D119:D120 D123 D126:D128 D130:D136 D3:D90</xm:sqref>
+          <xm:sqref>D94 D96:D106 D116:D119 D121:D122 D125 D128:D130 D132:D138 D3:D92</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>List!$A$4:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E92 E94:E104 E114:E117 E119:E120 E123 E126:E128 E130:E136 E3:E90</xm:sqref>
+          <xm:sqref>E94 E96:E106 E116:E119 E121:E122 E125 E128:E130 E132:E138 E3:E92</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>List!$D$5:$D$18</xm:f>
           </x14:formula1>
-          <xm:sqref>G126:G136 G119 G121 G123 G114:G117 G94:G98 G100:G104 G92 G90 G4:G88</xm:sqref>
+          <xm:sqref>G128:G138 G121 G123 G125 G116:G119 G96:G100 G102:G106 G94 G92 G4:G90</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>List!$D$3:$D$18</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G3 G89 G91 G93 G99 G120 G111:G113 G118 G105:G108 G122 G124:G125</xm:sqref>
+          <xm:sqref>G2:G3 G91 G93 G95 G101 G122 G113:G115 G120 G107:G110 G124 G126:G127</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>List!$D$3:$D$19</xm:f>
+          </x14:formula1>
+          <xm:sqref>G111:G112 G139:G141</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -4240,15 +4270,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>List!$D$3:$D$19</xm:f>
-          </x14:formula1>
-          <xm:sqref>G109:G110 G137:G139</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
             <xm:f>List!$H$2:$H$10</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B175</xm:sqref>
+          <xm:sqref>B2:B177</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4509,8 +4533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4625,6 +4649,12 @@
       <c r="F6" s="18" t="s">
         <v>252</v>
       </c>
+      <c r="H6" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -4650,7 +4680,9 @@
       <c r="D8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="31" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">

</xml_diff>